<commit_message>
Update fixtures loading error message
</commit_message>
<xml_diff>
--- a/EFL Grounds/The72.xlsx
+++ b/EFL Grounds/The72.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacMiniExternal/App Development/EFL-Grounds/EFL Grounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A97E5B-5A2A-414A-A2E8-8FCFEC5A31E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213FFF5-2F66-7F43-91A0-2C977AA7FFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{59B782F9-ABE7-C743-9AD6-7EE32320A32A}"/>
+    <workbookView xWindow="2620" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{59B782F9-ABE7-C743-9AD6-7EE32320A32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Leeds United</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>Chesterfield</t>
+  </si>
+  <si>
+    <t>Bromley</t>
   </si>
 </sst>
 </file>
@@ -642,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B7F621-C608-8E4F-9FFA-B95410D54F68}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -887,1351 +893,1393 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
+      <c r="A12" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>"Burton Albion</v>
+        <v>"Bromley</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>"Burton Albion"</v>
+        <v>"Bromley"</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
-        <v>"Burton Albion" {}</v>
+        <v>"Bromley" {}</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Burton Albion" {}</v>
+        <v>else if team == "Bromley" {}</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>"Cambridge United</v>
+        <v>"Burton Albion</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>"Cambridge United"</v>
+        <v>"Burton Albion"</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>"Cambridge United" {}</v>
+        <v>"Burton Albion" {}</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Cambridge United" {}</v>
+        <v>else if team == "Burton Albion" {}</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>"Cardiff City</v>
+        <v>"Cambridge United</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>"Cardiff City"</v>
+        <v>"Cambridge United"</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>"Cardiff City" {}</v>
+        <v>"Cambridge United" {}</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Cardiff City" {}</v>
+        <v>else if team == "Cambridge United" {}</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>"Carlisle United</v>
+        <v>"Cardiff City</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>"Carlisle United"</v>
+        <v>"Cardiff City"</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
-        <v>"Carlisle United" {}</v>
+        <v>"Cardiff City" {}</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Carlisle United" {}</v>
+        <v>else if team == "Cardiff City" {}</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>"Charlton Athletic</v>
+        <v>"Carlisle United</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>"Charlton Athletic"</v>
+        <v>"Carlisle United"</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
-        <v>"Charlton Athletic" {}</v>
+        <v>"Carlisle United" {}</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Charlton Athletic" {}</v>
+        <v>else if team == "Carlisle United" {}</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Charlton Athletic</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>"Charlton Athletic"</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>"Charlton Athletic" {}</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="3"/>
+        <v>else if team == "Charlton Athletic" {}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>"Cheltenham Town</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E18" t="str">
         <f t="shared" si="1"/>
         <v>"Cheltenham Town"</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="2"/>
         <v>"Cheltenham Town" {}</v>
       </c>
-      <c r="I17" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="3"/>
         <v>else if team == "Cheltenham Town" {}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>"Colchester United</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v>"Colchester United"</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="2"/>
-        <v>"Colchester United" {}</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="3"/>
-        <v>else if team == "Colchester United" {}</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>"Coventry City</v>
+        <v>"Chesterfield</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>"Coventry City"</v>
+        <v>"Chesterfield"</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="2"/>
-        <v>"Coventry City" {}</v>
+        <v>"Chesterfield" {}</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Coventry City" {}</v>
+        <v>else if team == "Chesterfield" {}</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="3" t="s">
-        <v>52</v>
+      <c r="A20" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>"Crawley Town</v>
+        <v>"Colchester United</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>"Crawley Town"</v>
+        <v>"Colchester United"</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
-        <v>"Crawley Town" {}</v>
+        <v>"Colchester United" {}</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Crawley Town" {}</v>
+        <v>else if team == "Colchester United" {}</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>"Crewe Alexandra</v>
+        <v>"Coventry City</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>"Crewe Alexandra"</v>
+        <v>"Coventry City"</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
-        <v>"Crewe Alexandra" {}</v>
+        <v>"Coventry City" {}</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Crewe Alexandra" {}</v>
+        <v>else if team == "Coventry City" {}</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>"Derby County</v>
+        <v>"Crawley Town</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>"Derby County"</v>
+        <v>"Crawley Town"</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
-        <v>"Derby County" {}</v>
+        <v>"Crawley Town" {}</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Derby County" {}</v>
+        <v>else if team == "Crawley Town" {}</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>"Doncaster Rovers</v>
+        <v>"Crewe Alexandra</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>"Doncaster Rovers"</v>
+        <v>"Crewe Alexandra"</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
-        <v>"Doncaster Rovers" {}</v>
+        <v>"Crewe Alexandra" {}</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Doncaster Rovers" {}</v>
+        <v>else if team == "Crewe Alexandra" {}</v>
       </c>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>"Exeter City</v>
+        <v>"Derby County</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>"Exeter City"</v>
+        <v>"Derby County"</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="2"/>
-        <v>"Exeter City" {}</v>
+        <v>"Derby County" {}</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Exeter City" {}</v>
+        <v>else if team == "Derby County" {}</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>"Fleetwood Town</v>
+        <v>"Doncaster Rovers</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>"Fleetwood Town"</v>
+        <v>"Doncaster Rovers"</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" t="str">
         <f t="shared" si="2"/>
-        <v>"Fleetwood Town" {}</v>
+        <v>"Doncaster Rovers" {}</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Fleetwood Town" {}</v>
+        <v>else if team == "Doncaster Rovers" {}</v>
       </c>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>"Gillingham</v>
+        <v>"Exeter City</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>"Gillingham"</v>
+        <v>"Exeter City"</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="2"/>
-        <v>"Gillingham" {}</v>
+        <v>"Exeter City" {}</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Gillingham" {}</v>
+        <v>else if team == "Exeter City" {}</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>"Grimsby Town</v>
+        <v>"Fleetwood Town</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>"Grimsby Town"</v>
+        <v>"Fleetwood Town"</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" t="str">
         <f t="shared" si="2"/>
-        <v>"Grimsby Town" {}</v>
+        <v>"Fleetwood Town" {}</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Grimsby Town" {}</v>
+        <v>else if team == "Fleetwood Town" {}</v>
       </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>"Harrogate Town</v>
+        <v>"Gillingham</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>"Harrogate Town"</v>
+        <v>"Gillingham"</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="2"/>
-        <v>"Harrogate Town" {}</v>
+        <v>"Gillingham" {}</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Harrogate Town" {}</v>
+        <v>else if team == "Gillingham" {}</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>"Huddersfield Town</v>
+        <v>"Grimsby Town</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>"Huddersfield Town"</v>
+        <v>"Grimsby Town"</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" t="str">
         <f t="shared" si="2"/>
-        <v>"Huddersfield Town" {}</v>
+        <v>"Grimsby Town" {}</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Huddersfield Town" {}</v>
+        <v>else if team == "Grimsby Town" {}</v>
       </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>"Hull City</v>
+        <v>"Harrogate Town</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>"Hull City"</v>
+        <v>"Harrogate Town"</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="2"/>
-        <v>"Hull City" {}</v>
+        <v>"Harrogate Town" {}</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Hull City" {}</v>
+        <v>else if team == "Harrogate Town" {}</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>"Leeds United</v>
+        <v>"Huddersfield Town</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>"Leeds United"</v>
+        <v>"Huddersfield Town"</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" t="str">
         <f t="shared" si="2"/>
-        <v>"Leeds United" {}</v>
+        <v>"Huddersfield Town" {}</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Leeds United" {}</v>
+        <v>else if team == "Huddersfield Town" {}</v>
       </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>"Leyton Orient</v>
+        <v>"Hull City</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>"Leyton Orient"</v>
+        <v>"Hull City"</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="2"/>
-        <v>"Leyton Orient" {}</v>
+        <v>"Hull City" {}</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Leyton Orient" {}</v>
+        <v>else if team == "Hull City" {}</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="3" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>"Lincoln City</v>
+        <v>"Leeds United</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>"Lincoln City"</v>
+        <v>"Leeds United"</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" t="str">
         <f t="shared" si="2"/>
-        <v>"Lincoln City" {}</v>
+        <v>"Leeds United" {}</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Lincoln City" {}</v>
+        <v>else if team == "Leeds United" {}</v>
       </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>"Mansfield Town</v>
+        <v>"Leyton Orient</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>"Mansfield Town"</v>
+        <v>"Leyton Orient"</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="2"/>
-        <v>"Mansfield Town" {}</v>
+        <v>"Leyton Orient" {}</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Mansfield Town" {}</v>
+        <v>else if team == "Leyton Orient" {}</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>"Middlesbrough</v>
+        <v>"Lincoln City</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>"Middlesbrough"</v>
+        <v>"Lincoln City"</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" t="str">
         <f t="shared" si="2"/>
-        <v>"Middlesbrough" {}</v>
+        <v>"Lincoln City" {}</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Middlesbrough" {}</v>
+        <v>else if team == "Lincoln City" {}</v>
       </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="3" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>"Millwall</v>
+        <v>"Mansfield Town</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>"Millwall"</v>
+        <v>"Mansfield Town"</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="2"/>
-        <v>"Millwall" {}</v>
+        <v>"Mansfield Town" {}</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Millwall" {}</v>
+        <v>else if team == "Mansfield Town" {}</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>"MK Dons</v>
+        <v>"Middlesbrough</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>"MK Dons"</v>
+        <v>"Middlesbrough"</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" t="str">
         <f t="shared" si="2"/>
-        <v>"MK Dons" {}</v>
+        <v>"Middlesbrough" {}</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "MK Dons" {}</v>
+        <v>else if team == "Middlesbrough" {}</v>
       </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>"Morecambe</v>
+        <v>"Millwall</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>"Morecambe"</v>
+        <v>"Millwall"</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="2"/>
-        <v>"Morecambe" {}</v>
+        <v>"Millwall" {}</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Morecambe" {}</v>
+        <v>else if team == "Millwall" {}</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>"Newport County</v>
+        <v>"MK Dons</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>"Newport County"</v>
+        <v>"MK Dons"</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" t="str">
         <f t="shared" si="2"/>
-        <v>"Newport County" {}</v>
+        <v>"MK Dons" {}</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Newport County" {}</v>
+        <v>else if team == "MK Dons" {}</v>
       </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="3" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>"Northampton Town</v>
+        <v>"Morecambe</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>"Northampton Town"</v>
+        <v>"Morecambe"</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="2"/>
-        <v>"Northampton Town" {}</v>
+        <v>"Morecambe" {}</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Northampton Town" {}</v>
+        <v>else if team == "Morecambe" {}</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>"Norwich City</v>
+        <v>"Newport County</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>"Norwich City"</v>
+        <v>"Newport County"</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" t="str">
         <f t="shared" si="2"/>
-        <v>"Norwich City" {}</v>
+        <v>"Newport County" {}</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Norwich City" {}</v>
+        <v>else if team == "Newport County" {}</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>"Notts County</v>
+        <v>"Northampton Town</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>"Notts County"</v>
+        <v>"Northampton Town"</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="2"/>
-        <v>"Notts County" {}</v>
+        <v>"Northampton Town" {}</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Notts County" {}</v>
+        <v>else if team == "Northampton Town" {}</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>"Oxford United</v>
+        <v>"Norwich City</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>"Oxford United"</v>
+        <v>"Norwich City"</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" t="str">
         <f t="shared" si="2"/>
-        <v>"Oxford United" {}</v>
+        <v>"Norwich City" {}</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Oxford United" {}</v>
+        <v>else if team == "Norwich City" {}</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="3" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>"Peterborough United</v>
+        <v>"Notts County</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>"Peterborough United"</v>
+        <v>"Notts County"</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="2"/>
-        <v>"Peterborough United" {}</v>
+        <v>"Notts County" {}</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Peterborough United" {}</v>
+        <v>else if team == "Notts County" {}</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>"Plymouth Argyle</v>
+        <v>"Oxford United</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>"Plymouth Argyle"</v>
+        <v>"Oxford United"</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" t="str">
         <f t="shared" si="2"/>
-        <v>"Plymouth Argyle" {}</v>
+        <v>"Oxford United" {}</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Plymouth Argyle" {}</v>
+        <v>else if team == "Oxford United" {}</v>
       </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>"Port Vale</v>
+        <v>"Peterborough United</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>"Port Vale"</v>
+        <v>"Peterborough United"</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="2"/>
-        <v>"Port Vale" {}</v>
+        <v>"Peterborough United" {}</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Port Vale" {}</v>
+        <v>else if team == "Peterborough United" {}</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>"Portsmouth</v>
+        <v>"Plymouth Argyle</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>"Portsmouth"</v>
+        <v>"Plymouth Argyle"</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" t="str">
         <f t="shared" si="2"/>
-        <v>"Portsmouth" {}</v>
+        <v>"Plymouth Argyle" {}</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Portsmouth" {}</v>
+        <v>else if team == "Plymouth Argyle" {}</v>
       </c>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="3" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>"Preston North End</v>
+        <v>"Port Vale</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>"Preston North End"</v>
+        <v>"Port Vale"</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="2"/>
-        <v>"Preston North End" {}</v>
+        <v>"Port Vale" {}</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Preston North End" {}</v>
+        <v>else if team == "Port Vale" {}</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>"Queens Park Rangers</v>
+        <v>"Portsmouth</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>"Queens Park Rangers"</v>
+        <v>"Portsmouth"</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" t="str">
         <f t="shared" si="2"/>
-        <v>"Queens Park Rangers" {}</v>
+        <v>"Portsmouth" {}</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Queens Park Rangers" {}</v>
+        <v>else if team == "Portsmouth" {}</v>
       </c>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>"Reading</v>
+        <v>"Preston North End</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>"Reading"</v>
+        <v>"Preston North End"</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="2"/>
-        <v>"Reading" {}</v>
+        <v>"Preston North End" {}</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Reading" {}</v>
+        <v>else if team == "Preston North End" {}</v>
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="4" t="s">
-        <v>21</v>
+      <c r="A51" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>"Rotherham United</v>
+        <v>"Queens Park Rangers</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>"Rotherham United"</v>
+        <v>"Queens Park Rangers"</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" t="str">
         <f t="shared" si="2"/>
-        <v>"Rotherham United" {}</v>
+        <v>"Queens Park Rangers" {}</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Rotherham United" {}</v>
+        <v>else if team == "Queens Park Rangers" {}</v>
       </c>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="3" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>"Salford City</v>
+        <v>"Reading</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>"Salford City"</v>
+        <v>"Reading"</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="2"/>
-        <v>"Salford City" {}</v>
+        <v>"Reading" {}</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Salford City" {}</v>
+        <v>else if team == "Reading" {}</v>
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="3" t="s">
-        <v>17</v>
+      <c r="A53" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>"Sheffield Wednesday</v>
+        <v>"Rotherham United</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>"Sheffield Wednesday"</v>
+        <v>"Rotherham United"</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" t="str">
         <f t="shared" si="2"/>
-        <v>"Sheffield Wednesday" {}</v>
+        <v>"Rotherham United" {}</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Sheffield Wednesday" {}</v>
+        <v>else if team == "Rotherham United" {}</v>
       </c>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>"Sheffield United</v>
+        <v>"Salford City</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>"Sheffield United"</v>
+        <v>"Salford City"</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" t="str">
         <f t="shared" si="2"/>
-        <v>"Sheffield United" {}</v>
+        <v>"Salford City" {}</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Sheffield United" {}</v>
+        <v>else if team == "Salford City" {}</v>
       </c>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="3" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>"Shrewsbury Town</v>
+        <v>"Sheffield United</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>"Shrewsbury Town"</v>
+        <v>"Sheffield United"</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="2"/>
-        <v>"Shrewsbury Town" {}</v>
+        <v>"Sheffield United" {}</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Shrewsbury Town" {}</v>
+        <v>else if team == "Sheffield United" {}</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>"Southampton</v>
+        <v>"Sheffield Wednesday</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>"Southampton"</v>
+        <v>"Sheffield Wednesday"</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" t="str">
         <f t="shared" si="2"/>
-        <v>"Southampton" {}</v>
+        <v>"Sheffield Wednesday" {}</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Southampton" {}</v>
+        <v>else if team == "Sheffield Wednesday" {}</v>
       </c>
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>"Stevenage</v>
+        <v>"Shrewsbury Town</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
-        <v>"Stevenage"</v>
+        <v>"Shrewsbury Town"</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="2"/>
-        <v>"Stevenage" {}</v>
+        <v>"Shrewsbury Town" {}</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Stevenage" {}</v>
+        <v>else if team == "Shrewsbury Town" {}</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="3" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>"Stockport County</v>
+        <v>"Southampton</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>"Stockport County"</v>
+        <v>"Southampton"</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" t="str">
         <f t="shared" si="2"/>
-        <v>"Stockport County" {}</v>
+        <v>"Southampton" {}</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Stockport County" {}</v>
+        <v>else if team == "Southampton" {}</v>
       </c>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>"Stoke City</v>
+        <v>"Stevenage</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
-        <v>"Stoke City"</v>
+        <v>"Stevenage"</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="2"/>
-        <v>"Stoke City" {}</v>
+        <v>"Stevenage" {}</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Stoke City" {}</v>
+        <v>else if team == "Stevenage" {}</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>"Sunderland</v>
+        <v>"Stockport County</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>"Sunderland"</v>
+        <v>"Stockport County"</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" t="str">
         <f t="shared" si="2"/>
-        <v>"Sunderland" {}</v>
+        <v>"Stockport County" {}</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Sunderland" {}</v>
+        <v>else if team == "Stockport County" {}</v>
       </c>
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>"Swansea City</v>
+        <v>"Stoke City</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
-        <v>"Swansea City"</v>
+        <v>"Stoke City"</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="2"/>
-        <v>"Swansea City" {}</v>
+        <v>"Stoke City" {}</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Swansea City" {}</v>
+        <v>else if team == "Stoke City" {}</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="3" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>"Swindon Town</v>
+        <v>"Sunderland</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
-        <v>"Swindon Town"</v>
+        <v>"Sunderland"</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" t="str">
         <f t="shared" si="2"/>
-        <v>"Swindon Town" {}</v>
+        <v>"Sunderland" {}</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Swindon Town" {}</v>
+        <v>else if team == "Sunderland" {}</v>
       </c>
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>"Tranmere Rovers</v>
+        <v>"Swansea City</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
-        <v>"Tranmere Rovers"</v>
+        <v>"Swansea City"</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="2"/>
-        <v>"Tranmere Rovers" {}</v>
+        <v>"Swansea City" {}</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Tranmere Rovers" {}</v>
+        <v>else if team == "Swansea City" {}</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>"Walsall</v>
+        <v>"Swindon Town</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
-        <v>"Walsall"</v>
+        <v>"Swindon Town"</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" t="str">
         <f t="shared" si="2"/>
-        <v>"Walsall" {}</v>
+        <v>"Swindon Town" {}</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Walsall" {}</v>
+        <v>else if team == "Swindon Town" {}</v>
       </c>
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="3" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v>"Watford</v>
+        <v>"Tranmere Rovers</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>"Watford"</v>
+        <v>"Tranmere Rovers"</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="2"/>
-        <v>"Watford" {}</v>
+        <v>"Tranmere Rovers" {}</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Watford" {}</v>
+        <v>else if team == "Tranmere Rovers" {}</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="3" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
-        <v>"West Bromwich Albion</v>
+        <v>"Walsall</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" t="str">
         <f t="shared" si="1"/>
-        <v>"West Bromwich Albion"</v>
+        <v>"Walsall"</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" t="str">
         <f t="shared" si="2"/>
-        <v>"West Bromwich Albion" {}</v>
+        <v>"Walsall" {}</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "West Bromwich Albion" {}</v>
+        <v>else if team == "Walsall" {}</v>
       </c>
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C69" si="4">_xlfn.CONCAT("""",A67)</f>
-        <v>"Wigan Athletic</v>
+        <f t="shared" ref="C67:C70" si="4">_xlfn.CONCAT("""",A67)</f>
+        <v>"Watford</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E69" si="5">_xlfn.CONCAT(C67,"""")</f>
-        <v>"Wigan Athletic"</v>
+        <f t="shared" ref="E67:E70" si="5">_xlfn.CONCAT(C67,"""")</f>
+        <v>"Watford"</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G69" si="6">_xlfn.CONCAT(E67, " {}")</f>
-        <v>"Wigan Athletic" {}</v>
+        <f t="shared" ref="G67:G70" si="6">_xlfn.CONCAT(E67, " {}")</f>
+        <v>"Watford" {}</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" si="3"/>
-        <v>else if team == "Wigan Athletic" {}</v>
+        <v>else if team == "Watford" {}</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="3" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" t="str">
         <f t="shared" si="4"/>
-        <v>"Wrexham</v>
+        <v>"West Bromwich Albion</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" t="str">
         <f t="shared" si="5"/>
-        <v>"Wrexham"</v>
+        <v>"West Bromwich Albion"</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" t="str">
         <f t="shared" si="6"/>
-        <v>"Wrexham" {}</v>
+        <v>"West Bromwich Albion" {}</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" t="str">
-        <f t="shared" ref="I68:I69" si="7">_xlfn.CONCAT("else if team == ",G68)</f>
-        <v>else if team == "Wrexham" {}</v>
+        <f t="shared" ref="I68:I70" si="7">_xlfn.CONCAT("else if team == ",G68)</f>
+        <v>else if team == "West Bromwich Albion" {}</v>
       </c>
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="4"/>
-        <v>"Wycombe Wanderers</v>
+        <v>"Wigan Athletic</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="5"/>
-        <v>"Wycombe Wanderers"</v>
+        <v>"Wigan Athletic"</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="6"/>
-        <v>"Wycombe Wanderers" {}</v>
+        <v>"Wigan Athletic" {}</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" si="7"/>
+        <v>else if team == "Wigan Athletic" {}</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" t="str">
+        <f t="shared" si="4"/>
+        <v>"Wrexham</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" t="str">
+        <f t="shared" si="5"/>
+        <v>"Wrexham"</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>"Wrexham" {}</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>else if team == "Wrexham" {}</v>
+      </c>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" ref="C71" si="8">_xlfn.CONCAT("""",A71)</f>
+        <v>"Wycombe Wanderers</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" t="str">
+        <f t="shared" ref="E71" si="9">_xlfn.CONCAT(C71,"""")</f>
+        <v>"Wycombe Wanderers"</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1" t="str">
+        <f t="shared" ref="G71" si="10">_xlfn.CONCAT(E71, " {}")</f>
+        <v>"Wycombe Wanderers" {}</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1" t="str">
+        <f t="shared" ref="I71" si="11">_xlfn.CONCAT("else if team == ",G71)</f>
         <v>else if team == "Wycombe Wanderers" {}</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="B70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
+      <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10" ht="19" customHeight="1">
       <c r="B72" s="1"/>
@@ -2438,8 +2486,8 @@
       <c r="B114" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A113">
-    <sortCondition ref="A1:A113"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A114">
+    <sortCondition ref="A48:A114"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>